<commit_message>
termine de tunear base debates, y base elecciones por ahora. segui probando modelo de elecciones, resultados interesantes
</commit_message>
<xml_diff>
--- a/tesis_doctorado/datav2023/base_anual_fullv2023.xlsx
+++ b/tesis_doctorado/datav2023/base_anual_fullv2023.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H187"/>
+  <dimension ref="A1:H192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -906,29 +906,29 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B20">
-        <v>1989</v>
+        <v>2023</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>1989</v>
+        <v>2015</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -938,7 +938,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>1993</v>
+        <v>1989</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -966,7 +966,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>2000</v>
+        <v>1993</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B25">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1106,7 +1106,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1130,17 +1130,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B28">
-        <v>1980</v>
+        <v>2021</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>1985</v>
+        <v>1980</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1190,10 +1190,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>1990</v>
+        <v>1985</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <v>1990</v>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="B31">
-        <v>1995</v>
+        <v>1990</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
         <v>1990</v>
@@ -1246,7 +1246,7 @@
         </is>
       </c>
       <c r="B32">
-        <v>2000</v>
+        <v>1995</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1274,10 +1274,10 @@
         </is>
       </c>
       <c r="B33">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>1990</v>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B34">
-        <v>2006</v>
+        <v>2001</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="B35">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1358,7 +1358,7 @@
         </is>
       </c>
       <c r="B36">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1386,7 +1386,7 @@
         </is>
       </c>
       <c r="B37">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1410,17 +1410,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B38">
-        <v>1989</v>
+        <v>2021</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1442,10 +1442,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>1993</v>
+        <v>1989</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <v>1993</v>
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="B40">
-        <v>1998</v>
+        <v>1993</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1498,7 +1498,7 @@
         </is>
       </c>
       <c r="B41">
-        <v>2003</v>
+        <v>1998</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="B42">
-        <v>2008</v>
+        <v>2003</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1554,7 +1554,7 @@
         </is>
       </c>
       <c r="B43">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B44">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1606,17 +1606,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B45">
-        <v>1960</v>
+        <v>2018</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>1979</v>
+        <v>1993</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1634,17 +1634,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B46">
-        <v>1966</v>
+        <v>2023</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>1979</v>
+        <v>1993</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1666,7 +1666,7 @@
         </is>
       </c>
       <c r="B47">
-        <v>1968</v>
+        <v>1960</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1694,10 +1694,10 @@
         </is>
       </c>
       <c r="B48">
-        <v>1979</v>
+        <v>1966</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>1979</v>
@@ -1722,10 +1722,10 @@
         </is>
       </c>
       <c r="B49">
-        <v>1984</v>
+        <v>1968</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49">
         <v>1979</v>
@@ -1750,10 +1750,10 @@
         </is>
       </c>
       <c r="B50">
-        <v>1988</v>
+        <v>1979</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>1979</v>
@@ -1778,7 +1778,7 @@
         </is>
       </c>
       <c r="B51">
-        <v>1992</v>
+        <v>1984</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1806,7 +1806,7 @@
         </is>
       </c>
       <c r="B52">
-        <v>1996</v>
+        <v>1988</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1834,10 +1834,10 @@
         </is>
       </c>
       <c r="B53">
-        <v>1998</v>
+        <v>1992</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
         <v>1979</v>
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="B54">
-        <v>2002</v>
+        <v>1996</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1890,10 +1890,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>2006</v>
+        <v>1998</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
         <v>1979</v>
@@ -1918,7 +1918,7 @@
         </is>
       </c>
       <c r="B56">
-        <v>2009</v>
+        <v>2002</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1927,16 +1927,16 @@
         <v>1979</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1946,7 +1946,7 @@
         </is>
       </c>
       <c r="B57">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1955,16 +1955,16 @@
         <v>1979</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1974,10 +1974,10 @@
         </is>
       </c>
       <c r="B58">
-        <v>2017</v>
+        <v>2009</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58">
         <v>1979</v>
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B59">
-        <v>2021</v>
+        <v>2013</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -2011,100 +2011,100 @@
         <v>1979</v>
       </c>
       <c r="E59">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F59">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
         <v>3</v>
-      </c>
-      <c r="H59">
-        <v>11</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B60">
-        <v>1984</v>
+        <v>2017</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>1984</v>
+        <v>1979</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B61">
-        <v>1989</v>
+        <v>2021</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>1984</v>
+        <v>1979</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B62">
-        <v>1994</v>
+        <v>2023</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>1984</v>
+        <v>1979</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63">
@@ -2114,10 +2114,10 @@
         </is>
       </c>
       <c r="B63">
-        <v>1999</v>
+        <v>1984</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>1984</v>
@@ -2142,10 +2142,10 @@
         </is>
       </c>
       <c r="B64">
-        <v>2004</v>
+        <v>1989</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>1984</v>
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="B65">
-        <v>2009</v>
+        <v>1994</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -2198,10 +2198,10 @@
         </is>
       </c>
       <c r="B66">
-        <v>2014</v>
+        <v>1999</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66">
         <v>1984</v>
@@ -2226,109 +2226,109 @@
         </is>
       </c>
       <c r="B67">
-        <v>2019</v>
+        <v>2004</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67">
         <v>1984</v>
       </c>
       <c r="E67">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B68">
+        <v>2009</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
         <v>1984</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-      <c r="D68">
-        <v>1990</v>
-      </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B69">
-        <v>1990</v>
+        <v>2014</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>1990</v>
+        <v>1984</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B70">
-        <v>1997</v>
+        <v>2019</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
-        <v>1990</v>
+        <v>1984</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71">
@@ -2338,7 +2338,7 @@
         </is>
       </c>
       <c r="B71">
-        <v>2001</v>
+        <v>1984</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2347,16 +2347,16 @@
         <v>1990</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -2366,7 +2366,7 @@
         </is>
       </c>
       <c r="B72">
-        <v>2006</v>
+        <v>1990</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2375,16 +2375,16 @@
         <v>1990</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
@@ -2394,7 +2394,7 @@
         </is>
       </c>
       <c r="B73">
-        <v>2011</v>
+        <v>1997</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="B74">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2446,17 +2446,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Nicaragua</t>
         </is>
       </c>
       <c r="B75">
-        <v>1994</v>
+        <v>2006</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>1994</v>
+        <v>1990</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -2474,17 +2474,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Nicaragua</t>
         </is>
       </c>
       <c r="B76">
-        <v>1999</v>
+        <v>2011</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76">
-        <v>1994</v>
+        <v>1990</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -2502,29 +2502,29 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Nicaragua</t>
         </is>
       </c>
       <c r="B77">
-        <v>2004</v>
+        <v>2016</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>1994</v>
+        <v>1990</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2534,7 +2534,7 @@
         </is>
       </c>
       <c r="B78">
-        <v>2009</v>
+        <v>1994</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -2543,16 +2543,16 @@
         <v>1994</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2562,25 +2562,25 @@
         </is>
       </c>
       <c r="B79">
-        <v>2014</v>
+        <v>1999</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79">
         <v>1994</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2590,7 +2590,7 @@
         </is>
       </c>
       <c r="B80">
-        <v>2019</v>
+        <v>2004</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -2599,100 +2599,100 @@
         <v>1994</v>
       </c>
       <c r="E80">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F80">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H80">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Venezuela</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="B81">
-        <v>1958</v>
+        <v>2009</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81">
-        <v>1963</v>
+        <v>1994</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Venezuela</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="B82">
-        <v>1963</v>
+        <v>2014</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82">
-        <v>1963</v>
+        <v>1994</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Venezuela</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="B83">
-        <v>1968</v>
+        <v>2019</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83">
-        <v>1963</v>
+        <v>1994</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84">
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="B84">
-        <v>1973</v>
+        <v>1958</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2730,10 +2730,10 @@
         </is>
       </c>
       <c r="B85">
-        <v>1978</v>
+        <v>1963</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85">
         <v>1963</v>
@@ -2758,7 +2758,7 @@
         </is>
       </c>
       <c r="B86">
-        <v>1983</v>
+        <v>1968</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -2786,7 +2786,7 @@
         </is>
       </c>
       <c r="B87">
-        <v>1988</v>
+        <v>1973</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2814,7 +2814,7 @@
         </is>
       </c>
       <c r="B88">
-        <v>1993</v>
+        <v>1978</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="B89">
-        <v>1998</v>
+        <v>1983</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -2870,7 +2870,7 @@
         </is>
       </c>
       <c r="B90">
-        <v>2000</v>
+        <v>1988</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2898,7 +2898,7 @@
         </is>
       </c>
       <c r="B91">
-        <v>2006</v>
+        <v>1993</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2926,10 +2926,10 @@
         </is>
       </c>
       <c r="B92">
-        <v>2012</v>
+        <v>1998</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92">
         <v>1963</v>
@@ -2954,7 +2954,7 @@
         </is>
       </c>
       <c r="B93">
-        <v>2013</v>
+        <v>2000</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="B94">
-        <v>2018</v>
+        <v>2006</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3006,17 +3006,17 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B95">
-        <v>1978</v>
+        <v>2012</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="D95">
-        <v>1989</v>
+        <v>1963</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -3034,17 +3034,17 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B96">
-        <v>1979</v>
+        <v>2013</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>1989</v>
+        <v>1963</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -3062,17 +3062,17 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="B97">
-        <v>1980</v>
+        <v>2018</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97">
-        <v>1989</v>
+        <v>1963</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -3094,7 +3094,7 @@
         </is>
       </c>
       <c r="B98">
-        <v>1985</v>
+        <v>1978</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -3122,10 +3122,10 @@
         </is>
       </c>
       <c r="B99">
-        <v>1989</v>
+        <v>1979</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99">
         <v>1989</v>
@@ -3150,10 +3150,10 @@
         </is>
       </c>
       <c r="B100">
-        <v>1993</v>
+        <v>1980</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100">
         <v>1989</v>
@@ -3178,10 +3178,10 @@
         </is>
       </c>
       <c r="B101">
-        <v>1997</v>
+        <v>1985</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101">
         <v>1989</v>
@@ -3206,7 +3206,7 @@
         </is>
       </c>
       <c r="B102">
-        <v>2002</v>
+        <v>1989</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -3234,7 +3234,7 @@
         </is>
       </c>
       <c r="B103">
-        <v>2005</v>
+        <v>1993</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -3262,10 +3262,10 @@
         </is>
       </c>
       <c r="B104">
-        <v>2009</v>
+        <v>1997</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D104">
         <v>1989</v>
@@ -3290,7 +3290,7 @@
         </is>
       </c>
       <c r="B105">
-        <v>2014</v>
+        <v>2002</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -3318,25 +3318,25 @@
         </is>
       </c>
       <c r="B106">
-        <v>2019</v>
+        <v>2005</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D106">
         <v>1989</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H106">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -3346,41 +3346,41 @@
         </is>
       </c>
       <c r="B107">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107">
         <v>1989</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B108">
-        <v>1982</v>
+        <v>2014</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108">
-        <v>1994</v>
+        <v>1989</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -3398,57 +3398,57 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B109">
-        <v>1988</v>
+        <v>2019</v>
       </c>
       <c r="C109">
         <v>0</v>
       </c>
       <c r="D109">
-        <v>1994</v>
+        <v>1989</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H109">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B110">
-        <v>1994</v>
+        <v>2020</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110">
-        <v>1994</v>
+        <v>1989</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G110">
         <v>1</v>
       </c>
       <c r="H110">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111">
@@ -3458,10 +3458,10 @@
         </is>
       </c>
       <c r="B111">
-        <v>2000</v>
+        <v>1982</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D111">
         <v>1994</v>
@@ -3470,13 +3470,13 @@
         <v>0</v>
       </c>
       <c r="F111">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G111">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H111">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -3486,10 +3486,10 @@
         </is>
       </c>
       <c r="B112">
-        <v>2006</v>
+        <v>1988</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D112">
         <v>1994</v>
@@ -3498,13 +3498,13 @@
         <v>0</v>
       </c>
       <c r="F112">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -3514,7 +3514,7 @@
         </is>
       </c>
       <c r="B113">
-        <v>2012</v>
+        <v>1994</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -3523,16 +3523,16 @@
         <v>1994</v>
       </c>
       <c r="E113">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F113">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H113">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="B114">
-        <v>2018</v>
+        <v>2000</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -3551,100 +3551,100 @@
         <v>1994</v>
       </c>
       <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
         <v>3</v>
-      </c>
-      <c r="F114">
-        <v>4</v>
       </c>
       <c r="G114">
         <v>2</v>
       </c>
       <c r="H114">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="B115">
-        <v>1966</v>
+        <v>2006</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D115">
-        <v>1985</v>
+        <v>1994</v>
       </c>
       <c r="E115">
         <v>0</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G115">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H115">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="B116">
-        <v>1970</v>
+        <v>2012</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D116">
-        <v>1985</v>
+        <v>1994</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F116">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G116">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H116">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="B117">
-        <v>1974</v>
+        <v>2018</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D117">
-        <v>1985</v>
+        <v>1994</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G117">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H117">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118">
@@ -3654,7 +3654,7 @@
         </is>
       </c>
       <c r="B118">
-        <v>1978</v>
+        <v>1966</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="B119">
-        <v>1982</v>
+        <v>1970</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -3710,10 +3710,10 @@
         </is>
       </c>
       <c r="B120">
-        <v>1985</v>
+        <v>1974</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D120">
         <v>1985</v>
@@ -3738,7 +3738,7 @@
         </is>
       </c>
       <c r="B121">
-        <v>1991</v>
+        <v>1978</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -3766,10 +3766,10 @@
         </is>
       </c>
       <c r="B122">
-        <v>1995</v>
+        <v>1982</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D122">
         <v>1985</v>
@@ -3794,7 +3794,7 @@
         </is>
       </c>
       <c r="B123">
-        <v>1999</v>
+        <v>1985</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="B124">
-        <v>2003</v>
+        <v>1990</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -3850,7 +3850,7 @@
         </is>
       </c>
       <c r="B125">
-        <v>2007</v>
+        <v>1995</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -3878,7 +3878,7 @@
         </is>
       </c>
       <c r="B126">
-        <v>2011</v>
+        <v>1999</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -3906,7 +3906,7 @@
         </is>
       </c>
       <c r="B127">
-        <v>2015</v>
+        <v>2003</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -3934,7 +3934,7 @@
         </is>
       </c>
       <c r="B128">
-        <v>2019</v>
+        <v>2007</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -3958,17 +3958,17 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="B129">
-        <v>1981</v>
+        <v>2011</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129">
-        <v>1993</v>
+        <v>1985</v>
       </c>
       <c r="E129">
         <v>0</v>
@@ -3986,17 +3986,17 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="B130">
+        <v>2015</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130">
         <v>1985</v>
-      </c>
-      <c r="C130">
-        <v>0</v>
-      </c>
-      <c r="D130">
-        <v>1993</v>
       </c>
       <c r="E130">
         <v>0</v>
@@ -4014,17 +4014,17 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="B131">
-        <v>1989</v>
+        <v>2019</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D131">
-        <v>1993</v>
+        <v>1985</v>
       </c>
       <c r="E131">
         <v>0</v>
@@ -4042,17 +4042,17 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="B132">
-        <v>1993</v>
+        <v>2023</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132">
-        <v>1993</v>
+        <v>1985</v>
       </c>
       <c r="E132">
         <v>0</v>
@@ -4074,10 +4074,10 @@
         </is>
       </c>
       <c r="B133">
-        <v>1997</v>
+        <v>1981</v>
       </c>
       <c r="C133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D133">
         <v>1993</v>
@@ -4102,10 +4102,10 @@
         </is>
       </c>
       <c r="B134">
-        <v>2001</v>
+        <v>1985</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D134">
         <v>1993</v>
@@ -4130,7 +4130,7 @@
         </is>
       </c>
       <c r="B135">
-        <v>2005</v>
+        <v>1989</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -4158,7 +4158,7 @@
         </is>
       </c>
       <c r="B136">
-        <v>2009</v>
+        <v>1993</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -4186,7 +4186,7 @@
         </is>
       </c>
       <c r="B137">
-        <v>2013</v>
+        <v>1997</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -4214,7 +4214,7 @@
         </is>
       </c>
       <c r="B138">
-        <v>2017</v>
+        <v>2001</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -4238,17 +4238,17 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="B139">
-        <v>1974</v>
+        <v>2005</v>
       </c>
       <c r="C139">
         <v>0</v>
       </c>
       <c r="D139">
-        <v>1986</v>
+        <v>1993</v>
       </c>
       <c r="E139">
         <v>0</v>
@@ -4266,17 +4266,17 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="B140">
-        <v>1978</v>
+        <v>2009</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D140">
-        <v>1986</v>
+        <v>1993</v>
       </c>
       <c r="E140">
         <v>0</v>
@@ -4294,17 +4294,17 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="B141">
-        <v>1982</v>
+        <v>2013</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D141">
-        <v>1986</v>
+        <v>1993</v>
       </c>
       <c r="E141">
         <v>0</v>
@@ -4322,17 +4322,17 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="B142">
-        <v>1986</v>
+        <v>2017</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142">
-        <v>1986</v>
+        <v>1993</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -4354,7 +4354,7 @@
         </is>
       </c>
       <c r="B143">
-        <v>1990</v>
+        <v>1974</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -4382,10 +4382,10 @@
         </is>
       </c>
       <c r="B144">
-        <v>1994</v>
+        <v>1978</v>
       </c>
       <c r="C144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D144">
         <v>1986</v>
@@ -4394,13 +4394,13 @@
         <v>0</v>
       </c>
       <c r="F144">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G144">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H144">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="B145">
-        <v>1998</v>
+        <v>1982</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D145">
         <v>1986</v>
@@ -4422,13 +4422,13 @@
         <v>0</v>
       </c>
       <c r="F145">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G145">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H145">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -4438,7 +4438,7 @@
         </is>
       </c>
       <c r="B146">
-        <v>2002</v>
+        <v>1986</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -4450,13 +4450,13 @@
         <v>0</v>
       </c>
       <c r="F146">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G146">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H146">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -4466,10 +4466,10 @@
         </is>
       </c>
       <c r="B147">
-        <v>2006</v>
+        <v>1990</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147">
         <v>1986</v>
@@ -4478,13 +4478,13 @@
         <v>0</v>
       </c>
       <c r="F147">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G147">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H147">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -4494,7 +4494,7 @@
         </is>
       </c>
       <c r="B148">
-        <v>2010</v>
+        <v>1994</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -4522,7 +4522,7 @@
         </is>
       </c>
       <c r="B149">
-        <v>2014</v>
+        <v>1998</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -4550,7 +4550,7 @@
         </is>
       </c>
       <c r="B150">
-        <v>2018</v>
+        <v>2002</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -4578,7 +4578,7 @@
         </is>
       </c>
       <c r="B151">
-        <v>2022</v>
+        <v>2006</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -4602,113 +4602,113 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B152">
-        <v>1962</v>
+        <v>2010</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D152">
-        <v>1978</v>
+        <v>1986</v>
       </c>
       <c r="E152">
         <v>0</v>
       </c>
       <c r="F152">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G152">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H152">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B153">
-        <v>1966</v>
+        <v>2014</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D153">
-        <v>1978</v>
+        <v>1986</v>
       </c>
       <c r="E153">
         <v>0</v>
       </c>
       <c r="F153">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G153">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H153">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B154">
-        <v>1970</v>
+        <v>2018</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D154">
-        <v>1978</v>
+        <v>1986</v>
       </c>
       <c r="E154">
         <v>0</v>
       </c>
       <c r="F154">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H154">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B155">
-        <v>1974</v>
+        <v>2022</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D155">
-        <v>1978</v>
+        <v>1986</v>
       </c>
       <c r="E155">
         <v>0</v>
       </c>
       <c r="F155">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G155">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H155">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156">
@@ -4718,10 +4718,10 @@
         </is>
       </c>
       <c r="B156">
-        <v>1978</v>
+        <v>1962</v>
       </c>
       <c r="C156">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D156">
         <v>1978</v>
@@ -4746,10 +4746,10 @@
         </is>
       </c>
       <c r="B157">
-        <v>1982</v>
+        <v>1966</v>
       </c>
       <c r="C157">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D157">
         <v>1978</v>
@@ -4774,10 +4774,10 @@
         </is>
       </c>
       <c r="B158">
-        <v>1986</v>
+        <v>1970</v>
       </c>
       <c r="C158">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D158">
         <v>1978</v>
@@ -4802,10 +4802,10 @@
         </is>
       </c>
       <c r="B159">
-        <v>1990</v>
+        <v>1974</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D159">
         <v>1978</v>
@@ -4830,7 +4830,7 @@
         </is>
       </c>
       <c r="B160">
-        <v>1994</v>
+        <v>1978</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -4858,7 +4858,7 @@
         </is>
       </c>
       <c r="B161">
-        <v>1998</v>
+        <v>1982</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -4867,16 +4867,16 @@
         <v>1978</v>
       </c>
       <c r="E161">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F161">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G161">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H161">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -4886,7 +4886,7 @@
         </is>
       </c>
       <c r="B162">
-        <v>2002</v>
+        <v>1986</v>
       </c>
       <c r="C162">
         <v>1</v>
@@ -4895,16 +4895,16 @@
         <v>1978</v>
       </c>
       <c r="E162">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F162">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G162">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H162">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -4914,7 +4914,7 @@
         </is>
       </c>
       <c r="B163">
-        <v>2006</v>
+        <v>1990</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -4923,16 +4923,16 @@
         <v>1978</v>
       </c>
       <c r="E163">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F163">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G163">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H163">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="B164">
-        <v>2010</v>
+        <v>1994</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -4951,16 +4951,16 @@
         <v>1978</v>
       </c>
       <c r="E164">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F164">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G164">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H164">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -4970,7 +4970,7 @@
         </is>
       </c>
       <c r="B165">
-        <v>2014</v>
+        <v>1998</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -4982,13 +4982,13 @@
         <v>3</v>
       </c>
       <c r="F165">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G165">
         <v>2</v>
       </c>
       <c r="H165">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166">
@@ -4998,7 +4998,7 @@
         </is>
       </c>
       <c r="B166">
-        <v>2018</v>
+        <v>2002</v>
       </c>
       <c r="C166">
         <v>1</v>
@@ -5010,13 +5010,13 @@
         <v>3</v>
       </c>
       <c r="F166">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G166">
         <v>2</v>
       </c>
       <c r="H166">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="167">
@@ -5026,7 +5026,7 @@
         </is>
       </c>
       <c r="B167">
-        <v>2022</v>
+        <v>2006</v>
       </c>
       <c r="C167">
         <v>1</v>
@@ -5038,125 +5038,125 @@
         <v>3</v>
       </c>
       <c r="F167">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G167">
         <v>2</v>
       </c>
       <c r="H167">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Republica Dominicana</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B168">
+        <v>2010</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168">
         <v>1978</v>
       </c>
-      <c r="C168">
-        <v>0</v>
-      </c>
-      <c r="D168">
-        <v>2016</v>
-      </c>
       <c r="E168">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F168">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G168">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H168">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Republica Dominicana</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B169">
-        <v>1982</v>
+        <v>2014</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D169">
-        <v>2016</v>
+        <v>1978</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F169">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G169">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H169">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Republica Dominicana</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B170">
-        <v>1986</v>
+        <v>2018</v>
       </c>
       <c r="C170">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D170">
-        <v>2016</v>
+        <v>1978</v>
       </c>
       <c r="E170">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F170">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G170">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H170">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Republica Dominicana</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B171">
-        <v>1990</v>
+        <v>2022</v>
       </c>
       <c r="C171">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D171">
-        <v>2016</v>
+        <v>1978</v>
       </c>
       <c r="E171">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F171">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G171">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H171">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="172">
@@ -5166,7 +5166,7 @@
         </is>
       </c>
       <c r="B172">
-        <v>1994</v>
+        <v>1978</v>
       </c>
       <c r="C172">
         <v>0</v>
@@ -5194,7 +5194,7 @@
         </is>
       </c>
       <c r="B173">
-        <v>1996</v>
+        <v>1982</v>
       </c>
       <c r="C173">
         <v>0</v>
@@ -5222,7 +5222,7 @@
         </is>
       </c>
       <c r="B174">
-        <v>2000</v>
+        <v>1986</v>
       </c>
       <c r="C174">
         <v>0</v>
@@ -5250,7 +5250,7 @@
         </is>
       </c>
       <c r="B175">
-        <v>2004</v>
+        <v>1990</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -5278,7 +5278,7 @@
         </is>
       </c>
       <c r="B176">
-        <v>2008</v>
+        <v>1994</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -5306,7 +5306,7 @@
         </is>
       </c>
       <c r="B177">
-        <v>2012</v>
+        <v>1996</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -5334,10 +5334,10 @@
         </is>
       </c>
       <c r="B178">
-        <v>2016</v>
+        <v>2000</v>
       </c>
       <c r="C178">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D178">
         <v>2016</v>
@@ -5362,7 +5362,7 @@
         </is>
       </c>
       <c r="B179">
-        <v>2020</v>
+        <v>2004</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -5374,29 +5374,29 @@
         <v>0</v>
       </c>
       <c r="F179">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G179">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H179">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>El Salvador</t>
+          <t>Republica Dominicana</t>
         </is>
       </c>
       <c r="B180">
-        <v>1984</v>
+        <v>2008</v>
       </c>
       <c r="C180">
         <v>0</v>
       </c>
       <c r="D180">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="E180">
         <v>0</v>
@@ -5414,17 +5414,17 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>El Salvador</t>
+          <t>Republica Dominicana</t>
         </is>
       </c>
       <c r="B181">
-        <v>1989</v>
+        <v>2012</v>
       </c>
       <c r="C181">
         <v>0</v>
       </c>
       <c r="D181">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="E181">
         <v>0</v>
@@ -5442,17 +5442,17 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>El Salvador</t>
+          <t>Republica Dominicana</t>
         </is>
       </c>
       <c r="B182">
-        <v>1994</v>
+        <v>2016</v>
       </c>
       <c r="C182">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D182">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="E182">
         <v>0</v>
@@ -5470,29 +5470,29 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>El Salvador</t>
+          <t>Republica Dominicana</t>
         </is>
       </c>
       <c r="B183">
-        <v>1999</v>
+        <v>2020</v>
       </c>
       <c r="C183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D183">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="E183">
         <v>0</v>
       </c>
       <c r="F183">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G183">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H183">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="184">
@@ -5502,7 +5502,7 @@
         </is>
       </c>
       <c r="B184">
-        <v>2004</v>
+        <v>1984</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -5530,7 +5530,7 @@
         </is>
       </c>
       <c r="B185">
-        <v>2009</v>
+        <v>1989</v>
       </c>
       <c r="C185">
         <v>0</v>
@@ -5558,10 +5558,10 @@
         </is>
       </c>
       <c r="B186">
-        <v>2014</v>
+        <v>1994</v>
       </c>
       <c r="C186">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D186">
         <v>1999</v>
@@ -5586,7 +5586,7 @@
         </is>
       </c>
       <c r="B187">
-        <v>2019</v>
+        <v>1999</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -5604,6 +5604,146 @@
         <v>0</v>
       </c>
       <c r="H187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B188">
+        <v>2004</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>1999</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B189">
+        <v>2009</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>1999</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B190">
+        <v>2014</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+      <c r="D190">
+        <v>1999</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
+      <c r="H190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B191">
+        <v>2019</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191">
+        <v>1999</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="B192">
+        <v>2024</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+      <c r="D192">
+        <v>1999</v>
+      </c>
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
         <v>0</v>
       </c>
     </row>

</xml_diff>